<commit_message>
Ajout de la prédiction TSP
</commit_message>
<xml_diff>
--- a/DATA DAP.xlsx
+++ b/DATA DAP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maha.laraki\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARYAM.BIROUK\MODEL PREDICTION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3864686-FFFD-410F-B164-872EA91DA5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F731286-666E-4C8F-9080-83BE5CC408A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{51288DA8-CBAC-4BFC-824C-9F2C46CC1047}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Période</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Prix DAP</t>
+  </si>
+  <si>
+    <t>Prix TSP</t>
   </si>
 </sst>
 </file>
@@ -159,42 +162,6 @@
   <dxfs count="4">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -230,16 +197,52 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color theme="1"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -256,23 +259,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BC98E25-5A36-46AB-985F-8C2B3D2C2991}" name="Tableau1" displayName="Tableau1" ref="A1:E49" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
-  <autoFilter ref="A1:E49" xr:uid="{4BC98E25-5A36-46AB-985F-8C2B3D2C2991}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2CCE69B4-BCAD-4E5D-84CE-0E16200749B2}" name="Période" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BC98E25-5A36-46AB-985F-8C2B3D2C2991}" name="Tableau1" displayName="Tableau1" ref="A1:F49" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:F49" xr:uid="{4BC98E25-5A36-46AB-985F-8C2B3D2C2991}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2CCE69B4-BCAD-4E5D-84CE-0E16200749B2}" name="Période" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{06C1152F-D6F2-46D9-83FD-0FDFEACDF8BD}" name="Prix DAP"/>
     <tableColumn id="3" xr3:uid="{1A54B0D6-D59C-4598-99E7-3548D1CD493A}" name="Prix Soufre"/>
     <tableColumn id="4" xr3:uid="{E8D8E46B-D82C-4C13-AD51-C9EF16C8E17B}" name="Prix NH3"/>
     <tableColumn id="5" xr3:uid="{8D44BC49-0609-4AE4-B932-87EEBBF1F322}" name="Prix ACS"/>
+    <tableColumn id="6" xr3:uid="{9C4B7F7C-BF0B-4FC8-B1CE-979BE5116D4E}" name="Prix TSP"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -310,7 +314,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -416,7 +420,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -558,7 +562,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -566,18 +570,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40330A1-C608-47CA-BFEE-AD4C7851D203}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="11.90625" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -593,8 +598,11 @@
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44197</v>
       </c>
@@ -610,8 +618,11 @@
       <c r="E2">
         <v>34.47883814704992</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>267.74737611748355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44228</v>
       </c>
@@ -627,8 +638,11 @@
       <c r="E3">
         <v>35.293766078522438</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>320.50615838606103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44256</v>
       </c>
@@ -644,8 +658,11 @@
       <c r="E4">
         <v>90.713025500402964</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>335.36322723603217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44287</v>
       </c>
@@ -661,8 +678,11 @@
       <c r="E5">
         <v>83.229773104504645</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>411.58927879408168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44317</v>
       </c>
@@ -678,8 +698,11 @@
       <c r="E6">
         <v>87.291321371928532</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>481.93721062003419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44348</v>
       </c>
@@ -695,8 +718,11 @@
       <c r="E7">
         <v>163.04185538127555</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>493.58760761581902</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44378</v>
       </c>
@@ -712,8 +738,11 @@
       <c r="E8">
         <v>157.68041390570971</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>538.67783908274714</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44409</v>
       </c>
@@ -729,8 +758,11 @@
       <c r="E9">
         <v>162.36929711834105</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>619.81446658599202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44440</v>
       </c>
@@ -746,8 +778,11 @@
       <c r="E10">
         <v>189.14525896897021</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>583.17754284926309</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44470</v>
       </c>
@@ -763,8 +798,11 @@
       <c r="E11">
         <v>159.16772974941608</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>547.08557077308285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44501</v>
       </c>
@@ -780,8 +818,11 @@
       <c r="E12">
         <v>260.33724520708734</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <v>606.38191056603966</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44531</v>
       </c>
@@ -797,8 +838,11 @@
       <c r="E13">
         <v>208.31623596701402</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>644.12187851407236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44562</v>
       </c>
@@ -814,8 +858,11 @@
       <c r="E14">
         <v>233.22152113074188</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <v>701.13260620976212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44593</v>
       </c>
@@ -831,8 +878,11 @@
       <c r="E15">
         <v>204.5191761221258</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>44621</v>
       </c>
@@ -848,8 +898,11 @@
       <c r="E16">
         <v>244.24356377779216</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <v>700.64750792612949</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44652</v>
       </c>
@@ -865,8 +918,11 @@
       <c r="E17">
         <v>222.88475497498897</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <v>903.49661935509459</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>44682</v>
       </c>
@@ -882,8 +938,11 @@
       <c r="E18">
         <v>201.42768931586096</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <v>970.96058802397135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>44713</v>
       </c>
@@ -899,8 +958,11 @@
       <c r="E19">
         <v>219.29055498390846</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <v>717.76783814089595</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>44743</v>
       </c>
@@ -916,8 +978,11 @@
       <c r="E20">
         <v>245.26108949751375</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <v>721.78502775499192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>44774</v>
       </c>
@@ -933,8 +998,11 @@
       <c r="E21">
         <v>238.10440361209476</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21">
+        <v>785.74556336099408</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>44805</v>
       </c>
@@ -950,8 +1018,11 @@
       <c r="E22">
         <v>265.60123779019614</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22">
+        <v>693.43033122426732</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>44835</v>
       </c>
@@ -967,8 +1038,11 @@
       <c r="E23">
         <v>113.66039977156626</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23">
+        <v>661.2415008512379</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>44866</v>
       </c>
@@ -984,8 +1058,11 @@
       <c r="E24">
         <v>96.494011863135484</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24">
+        <v>387.16212765957448</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>44896</v>
       </c>
@@ -998,8 +1075,11 @@
       <c r="D25">
         <v>1063.1661429551523</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25">
+        <v>439.59987941469245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>44927</v>
       </c>
@@ -1015,8 +1095,11 @@
       <c r="E26">
         <v>38.187144468743192</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26">
+        <v>473.7031495401406</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>44958</v>
       </c>
@@ -1032,8 +1115,11 @@
       <c r="E27">
         <v>74.462889608704884</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27">
+        <v>443.04752604764099</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>44986</v>
       </c>
@@ -1049,8 +1135,11 @@
       <c r="E28">
         <v>66.808020607714283</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28">
+        <v>383.01967167590209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45017</v>
       </c>
@@ -1063,8 +1152,11 @@
       <c r="D29">
         <v>516.56588428529233</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29">
+        <v>384.37074369159416</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45047</v>
       </c>
@@ -1077,8 +1169,11 @@
       <c r="D30">
         <v>402.60035375787339</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30">
+        <v>380.52525067592018</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45078</v>
       </c>
@@ -1094,8 +1189,11 @@
       <c r="E31">
         <v>59.953557988199123</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31">
+        <v>331.99481299422956</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>45108</v>
       </c>
@@ -1108,8 +1206,11 @@
       <c r="D32">
         <v>305.98411148035837</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32">
+        <v>342.00988593704562</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>45139</v>
       </c>
@@ -1125,8 +1226,11 @@
       <c r="E33">
         <v>61.456187558930765</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33">
+        <v>339.80463588897572</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>45170</v>
       </c>
@@ -1142,8 +1246,11 @@
       <c r="E34">
         <v>75.297929518772165</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34">
+        <v>376.09120144127439</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>45200</v>
       </c>
@@ -1159,8 +1266,11 @@
       <c r="E35">
         <v>88.122109051273</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35">
+        <v>396.24926974395703</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>45231</v>
       </c>
@@ -1176,8 +1286,11 @@
       <c r="E36">
         <v>108.90451340725451</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36">
+        <v>401.7686977749708</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>45261</v>
       </c>
@@ -1193,8 +1306,11 @@
       <c r="E37">
         <v>117.45127898126781</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37">
+        <v>398.20689444428109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>45292</v>
       </c>
@@ -1210,8 +1326,11 @@
       <c r="E38">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38">
+        <v>406.14347451452056</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>45323</v>
       </c>
@@ -1227,8 +1346,11 @@
       <c r="E39">
         <v>81</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39">
+        <v>397.24050742441119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>45352</v>
       </c>
@@ -1244,8 +1366,11 @@
       <c r="E40">
         <v>83</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40">
+        <v>395.91180800645901</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>45383</v>
       </c>
@@ -1261,8 +1386,11 @@
       <c r="E41">
         <v>108</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41">
+        <v>358.73110949800457</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>45413</v>
       </c>
@@ -1278,8 +1406,11 @@
       <c r="E42">
         <v>116</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42">
+        <v>381.68920664576007</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>45444</v>
       </c>
@@ -1295,8 +1426,11 @@
       <c r="E43">
         <v>131</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43">
+        <v>384.25059914910969</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>45474</v>
       </c>
@@ -1312,8 +1446,11 @@
       <c r="E44">
         <v>135</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44">
+        <v>380.15482969888251</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>45505</v>
       </c>
@@ -1329,8 +1466,11 @@
       <c r="E45">
         <v>134</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45">
+        <v>412.59185125703368</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45536</v>
       </c>
@@ -1346,8 +1486,11 @@
       <c r="E46">
         <v>149</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F46">
+        <v>428.32217072847618</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>45566</v>
       </c>
@@ -1363,8 +1506,11 @@
       <c r="E47">
         <v>142</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F47">
+        <v>431.42029846944047</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>45597</v>
       </c>
@@ -1380,8 +1526,11 @@
       <c r="E48">
         <v>134</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48">
+        <v>422.64952432346183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>45627</v>
       </c>
@@ -1396,6 +1545,9 @@
       </c>
       <c r="E49">
         <v>142</v>
+      </c>
+      <c r="F49">
+        <v>436.99855262881238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>